<commit_message>
PL-EQ - Level 2 Integration: Improvements & Fixes  - Iteration 35
</commit_message>
<xml_diff>
--- a/tests/Feature/Data/opportunity/opps-23032022.xlsx
+++ b/tests/Feature/Data/opportunity/opps-23032022.xlsx
@@ -250,7 +250,7 @@
     <t xml:space="preserve">Various</t>
   </si>
   <si>
-    <t xml:space="preserve">Worldwide</t>
+    <t xml:space="preserve">DEV</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -484,11 +484,11 @@
   </sheetPr>
   <dimension ref="A1:BU1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AQ5" activeCellId="0" sqref="AQ5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="1" style="0" width="15.71"/>
   </cols>
@@ -1540,8 +1540,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>